<commit_message>
commit file throug Batch
</commit_message>
<xml_diff>
--- a/doc/BookList.xlsx
+++ b/doc/BookList.xlsx
@@ -1196,7 +1196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1204,6 +1204,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1511,8 +1514,8 @@
   <dimension ref="A1:D266"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A259" sqref="A259:D259"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1520,7 +1523,7 @@
     <col min="1" max="1" width="13.625" customWidth="1"/>
     <col min="2" max="2" width="38.25" customWidth="1"/>
     <col min="3" max="3" width="14.25" customWidth="1"/>
-    <col min="4" max="4" width="33.875" customWidth="1"/>
+    <col min="4" max="4" width="49.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
@@ -2642,14 +2645,14 @@
       <c r="C207" s="4"/>
       <c r="D207" s="4"/>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:4" ht="54" x14ac:dyDescent="0.15">
       <c r="B208" t="s">
         <v>34</v>
       </c>
       <c r="C208" t="s">
         <v>115</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D208" s="5" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2657,43 +2660,47 @@
       <c r="B209" t="s">
         <v>35</v>
       </c>
+      <c r="D209" s="5"/>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B210" t="s">
         <v>36</v>
       </c>
+      <c r="D210" s="5"/>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B211" t="s">
         <v>37</v>
       </c>
+      <c r="D211" s="5"/>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B212" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D212" s="5"/>
+    </row>
+    <row r="213" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B213" t="s">
         <v>30</v>
       </c>
-      <c r="D213" t="s">
+      <c r="D213" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B214" t="s">
         <v>31</v>
       </c>
-      <c r="D214" t="s">
+      <c r="D214" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B215" t="s">
         <v>32</v>
       </c>
-      <c r="D215" t="s">
+      <c r="D215" s="5" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2704,7 +2711,7 @@
       <c r="C216" t="s">
         <v>114</v>
       </c>
-      <c r="D216" t="s">
+      <c r="D216" s="5" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2975,27 +2982,30 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A139:D139"/>
+    <mergeCell ref="A112:D112"/>
+    <mergeCell ref="A142:D142"/>
+    <mergeCell ref="A148:D148"/>
+    <mergeCell ref="A154:D154"/>
+    <mergeCell ref="A158:D158"/>
+    <mergeCell ref="A184:D184"/>
     <mergeCell ref="A259:D259"/>
     <mergeCell ref="A207:D207"/>
     <mergeCell ref="A221:D221"/>
     <mergeCell ref="A227:D227"/>
     <mergeCell ref="A232:D232"/>
     <mergeCell ref="A245:D245"/>
-    <mergeCell ref="A142:D142"/>
-    <mergeCell ref="A148:D148"/>
-    <mergeCell ref="A154:D154"/>
-    <mergeCell ref="A158:D158"/>
-    <mergeCell ref="A184:D184"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A139:D139"/>
-    <mergeCell ref="A112:D112"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <webPublishItems count="1">
+    <webPublishItem id="27433" divId="BookList_27433" sourceType="sheet" destinationFile="G:\Projects\jacksoncode.github.io\doc\BookList.htm"/>
+  </webPublishItems>
 </worksheet>
 </file>
 

</xml_diff>